<commit_message>
action probability based on id_building_ownership added
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_Building_Ownership.xlsx
+++ b/projects/test_building/input/ID_Building_Ownership.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD570869-1723-8745-8A23-D5C93565A873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91865C1D-1365-BD4C-AEE2-4DE1F6B22DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="-18080" windowWidth="27240" windowHeight="16400" xr2:uid="{936E5B29-2ED2-0B46-BBCD-4B6DD664E122}"/>
+    <workbookView xWindow="5600" yWindow="-20860" windowWidth="20400" windowHeight="13820" xr2:uid="{936E5B29-2ED2-0B46-BBCD-4B6DD664E122}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>